<commit_message>
BrazilCFR: Adding lags and volatility window
</commit_message>
<xml_diff>
--- a/DataFeeds/TotalFertilizerProduction.xlsx
+++ b/DataFeeds/TotalFertilizerProduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmpMeesam\Dev\Canpotex\DataFeeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C40B4E6E-64D7-4980-87EC-515FDFB7C8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3F1F8B-A8B8-47BF-8BE1-B14C568DE554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{AEDBEFD4-77D7-4A40-BF43-C035E530B386}"/>
+    <workbookView xWindow="-24110" yWindow="2460" windowWidth="24220" windowHeight="13120" xr2:uid="{AEDBEFD4-77D7-4A40-BF43-C035E530B386}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,18 +392,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C442087-E244-447E-BFE7-392C51ACDEAA}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -410,59 +411,635 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2016</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>42370</v>
       </c>
       <c r="B2">
         <v>244131</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2017</v>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>42401</v>
       </c>
       <c r="B3">
-        <v>249101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2018</v>
+        <v>244131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>42430</v>
       </c>
       <c r="B4">
-        <v>255861</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2019</v>
+        <v>244131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>42461</v>
       </c>
       <c r="B5">
-        <v>262387</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2020</v>
+        <v>244131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>42491</v>
       </c>
       <c r="B6">
-        <v>263764</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2021</v>
+        <v>244131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>42522</v>
       </c>
       <c r="B7">
-        <v>266756</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2022</v>
+        <v>244131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>42552</v>
       </c>
       <c r="B8">
+        <v>244131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>42583</v>
+      </c>
+      <c r="B9">
+        <v>244131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>42614</v>
+      </c>
+      <c r="B10">
+        <v>244131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>42644</v>
+      </c>
+      <c r="B11">
+        <v>244131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>42675</v>
+      </c>
+      <c r="B12">
+        <v>244131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>42705</v>
+      </c>
+      <c r="B13">
+        <v>244131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>42736</v>
+      </c>
+      <c r="B14">
+        <v>249101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>42767</v>
+      </c>
+      <c r="B15">
+        <v>249101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>42795</v>
+      </c>
+      <c r="B16">
+        <v>249101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>42826</v>
+      </c>
+      <c r="B17">
+        <v>249101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>42856</v>
+      </c>
+      <c r="B18">
+        <v>249101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>42887</v>
+      </c>
+      <c r="B19">
+        <v>249101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>42917</v>
+      </c>
+      <c r="B20">
+        <v>249101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>42948</v>
+      </c>
+      <c r="B21">
+        <v>249101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>42979</v>
+      </c>
+      <c r="B22">
+        <v>249101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>43009</v>
+      </c>
+      <c r="B23">
+        <v>249101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>43040</v>
+      </c>
+      <c r="B24">
+        <v>249101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>43070</v>
+      </c>
+      <c r="B25">
+        <v>249101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>43101</v>
+      </c>
+      <c r="B26">
+        <v>255861</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>43132</v>
+      </c>
+      <c r="B27">
+        <v>255861</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>43160</v>
+      </c>
+      <c r="B28">
+        <v>255861</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>43191</v>
+      </c>
+      <c r="B29">
+        <v>255861</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>43221</v>
+      </c>
+      <c r="B30">
+        <v>255861</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>43252</v>
+      </c>
+      <c r="B31">
+        <v>255861</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>43282</v>
+      </c>
+      <c r="B32">
+        <v>255861</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>43313</v>
+      </c>
+      <c r="B33">
+        <v>255861</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>43344</v>
+      </c>
+      <c r="B34">
+        <v>255861</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>43374</v>
+      </c>
+      <c r="B35">
+        <v>255861</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>43405</v>
+      </c>
+      <c r="B36">
+        <v>255861</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>43435</v>
+      </c>
+      <c r="B37">
+        <v>255861</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B38">
+        <v>262387</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>43497</v>
+      </c>
+      <c r="B39">
+        <v>262387</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>43525</v>
+      </c>
+      <c r="B40">
+        <v>262387</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <v>43556</v>
+      </c>
+      <c r="B41">
+        <v>262387</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>43586</v>
+      </c>
+      <c r="B42">
+        <v>262387</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
+        <v>43617</v>
+      </c>
+      <c r="B43">
+        <v>262387</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <v>43647</v>
+      </c>
+      <c r="B44">
+        <v>262387</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>43678</v>
+      </c>
+      <c r="B45">
+        <v>262387</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>43709</v>
+      </c>
+      <c r="B46">
+        <v>262387</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>43739</v>
+      </c>
+      <c r="B47">
+        <v>262387</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>43770</v>
+      </c>
+      <c r="B48">
+        <v>262387</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>43800</v>
+      </c>
+      <c r="B49">
+        <v>262387</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B50">
+        <v>263764</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>43862</v>
+      </c>
+      <c r="B51">
+        <v>263764</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>43891</v>
+      </c>
+      <c r="B52">
+        <v>263764</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B53">
+        <v>263764</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B54">
+        <v>263764</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B55">
+        <v>263764</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B56">
+        <v>263764</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B57">
+        <v>263764</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B58">
+        <v>263764</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B59">
+        <v>263764</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B60">
+        <v>263764</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B61">
+        <v>263764</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B62">
+        <v>266756</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B63">
+        <v>266756</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B64">
+        <v>266756</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B65">
+        <v>266756</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B66">
+        <v>266756</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B67">
+        <v>266756</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B68">
+        <v>266756</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B69">
+        <v>266756</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B70">
+        <v>266756</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B71">
+        <v>266756</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B72">
+        <v>266756</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B73">
+        <v>266756</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B74">
+        <v>269482</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B75">
+        <v>269482</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B76">
+        <v>269482</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B77">
+        <v>269482</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B78">
+        <v>269482</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B79">
+        <v>269482</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B80">
         <v>269482</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Creating backester and distribution calculator
</commit_message>
<xml_diff>
--- a/DataFeeds/TotalFertilizerProduction.xlsx
+++ b/DataFeeds/TotalFertilizerProduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmpMeesam\Dev\Canpotex\DataFeeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3F1F8B-A8B8-47BF-8BE1-B14C568DE554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A073DD2-C10F-4817-B02D-79957226683F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24110" yWindow="2460" windowWidth="24220" windowHeight="13120" xr2:uid="{AEDBEFD4-77D7-4A40-BF43-C035E530B386}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AEDBEFD4-77D7-4A40-BF43-C035E530B386}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,655 +398,1425 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C442087-E244-447E-BFE7-392C51ACDEAA}">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:B176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B80"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B19" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>42370</v>
-      </c>
-      <c r="B2">
-        <v>244131</v>
+        <v>39448</v>
+      </c>
+      <c r="B2" s="2">
+        <v>166570350.69999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>42401</v>
-      </c>
-      <c r="B3">
-        <v>244131</v>
+        <v>39479</v>
+      </c>
+      <c r="B3" s="2">
+        <v>166570350.69999999</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>42430</v>
-      </c>
-      <c r="B4">
-        <v>244131</v>
+        <v>39508</v>
+      </c>
+      <c r="B4" s="2">
+        <v>166570350.69999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>42461</v>
-      </c>
-      <c r="B5">
-        <v>244131</v>
+        <v>39539</v>
+      </c>
+      <c r="B5" s="2">
+        <v>166570350.69999999</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>42491</v>
-      </c>
-      <c r="B6">
-        <v>244131</v>
+        <v>39569</v>
+      </c>
+      <c r="B6" s="2">
+        <v>166570350.69999999</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>42522</v>
-      </c>
-      <c r="B7">
-        <v>244131</v>
+        <v>39600</v>
+      </c>
+      <c r="B7" s="2">
+        <v>166570350.69999999</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>42552</v>
-      </c>
-      <c r="B8">
-        <v>244131</v>
+        <v>39630</v>
+      </c>
+      <c r="B8" s="2">
+        <v>166570350.69999999</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>42583</v>
-      </c>
-      <c r="B9">
-        <v>244131</v>
+        <v>39661</v>
+      </c>
+      <c r="B9" s="2">
+        <v>166570350.69999999</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>42614</v>
-      </c>
-      <c r="B10">
-        <v>244131</v>
+        <v>39692</v>
+      </c>
+      <c r="B10" s="2">
+        <v>166570350.69999999</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>42644</v>
-      </c>
-      <c r="B11">
-        <v>244131</v>
+        <v>39722</v>
+      </c>
+      <c r="B11" s="2">
+        <v>166570350.69999999</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>42675</v>
-      </c>
-      <c r="B12">
-        <v>244131</v>
+        <v>39753</v>
+      </c>
+      <c r="B12" s="2">
+        <v>166570350.69999999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>42705</v>
-      </c>
-      <c r="B13">
-        <v>244131</v>
+        <v>39783</v>
+      </c>
+      <c r="B13" s="2">
+        <v>166570350.69999999</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>42736</v>
-      </c>
-      <c r="B14">
-        <v>249101</v>
+        <v>39814</v>
+      </c>
+      <c r="B14" s="2">
+        <v>157176670.97</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>42767</v>
-      </c>
-      <c r="B15">
-        <v>249101</v>
+        <v>39845</v>
+      </c>
+      <c r="B15" s="2">
+        <v>157176670.97</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>42795</v>
-      </c>
-      <c r="B16">
-        <v>249101</v>
+        <v>39873</v>
+      </c>
+      <c r="B16" s="2">
+        <v>157176670.97</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>42826</v>
-      </c>
-      <c r="B17">
-        <v>249101</v>
+        <v>39904</v>
+      </c>
+      <c r="B17" s="2">
+        <v>157176670.97</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>42856</v>
-      </c>
-      <c r="B18">
-        <v>249101</v>
+        <v>39934</v>
+      </c>
+      <c r="B18" s="2">
+        <v>157176670.97</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>42887</v>
-      </c>
-      <c r="B19">
-        <v>249101</v>
+        <v>39965</v>
+      </c>
+      <c r="B19" s="2">
+        <v>157176670.97</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>42917</v>
-      </c>
-      <c r="B20">
-        <v>249101</v>
+        <v>39995</v>
+      </c>
+      <c r="B20" s="2">
+        <v>157176670.97</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>42948</v>
-      </c>
-      <c r="B21">
-        <v>249101</v>
+        <v>40026</v>
+      </c>
+      <c r="B21" s="2">
+        <v>157176670.97</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>42979</v>
-      </c>
-      <c r="B22">
-        <v>249101</v>
+        <v>40057</v>
+      </c>
+      <c r="B22" s="2">
+        <v>157176670.97</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>43009</v>
-      </c>
-      <c r="B23">
-        <v>249101</v>
+        <v>40087</v>
+      </c>
+      <c r="B23" s="2">
+        <v>157176670.97</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>43040</v>
-      </c>
-      <c r="B24">
-        <v>249101</v>
+        <v>40118</v>
+      </c>
+      <c r="B24" s="2">
+        <v>157176670.97</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>43070</v>
-      </c>
-      <c r="B25">
-        <v>249101</v>
+        <v>40148</v>
+      </c>
+      <c r="B25" s="2">
+        <v>157176670.97</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>43101</v>
-      </c>
-      <c r="B26">
-        <v>255861</v>
+        <v>40179</v>
+      </c>
+      <c r="B26" s="2">
+        <v>186546890.25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>43132</v>
-      </c>
-      <c r="B27">
-        <v>255861</v>
+        <v>40210</v>
+      </c>
+      <c r="B27" s="2">
+        <v>186546890.25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>43160</v>
-      </c>
-      <c r="B28">
-        <v>255861</v>
+        <v>40238</v>
+      </c>
+      <c r="B28" s="2">
+        <v>186546890.25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>43191</v>
-      </c>
-      <c r="B29">
-        <v>255861</v>
+        <v>40269</v>
+      </c>
+      <c r="B29" s="2">
+        <v>186546890.25</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>43221</v>
-      </c>
-      <c r="B30">
-        <v>255861</v>
+        <v>40299</v>
+      </c>
+      <c r="B30" s="2">
+        <v>186546890.25</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>43252</v>
-      </c>
-      <c r="B31">
-        <v>255861</v>
+        <v>40330</v>
+      </c>
+      <c r="B31" s="2">
+        <v>186546890.25</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>43282</v>
-      </c>
-      <c r="B32">
-        <v>255861</v>
+        <v>40360</v>
+      </c>
+      <c r="B32" s="2">
+        <v>186546890.25</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>43313</v>
-      </c>
-      <c r="B33">
-        <v>255861</v>
+        <v>40391</v>
+      </c>
+      <c r="B33" s="2">
+        <v>186546890.25</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>43344</v>
-      </c>
-      <c r="B34">
-        <v>255861</v>
+        <v>40422</v>
+      </c>
+      <c r="B34" s="2">
+        <v>186546890.25</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>43374</v>
-      </c>
-      <c r="B35">
-        <v>255861</v>
+        <v>40452</v>
+      </c>
+      <c r="B35" s="2">
+        <v>186546890.25</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>43405</v>
-      </c>
-      <c r="B36">
-        <v>255861</v>
+        <v>40483</v>
+      </c>
+      <c r="B36" s="2">
+        <v>186546890.25</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>43435</v>
-      </c>
-      <c r="B37">
-        <v>255861</v>
+        <v>40513</v>
+      </c>
+      <c r="B37" s="2">
+        <v>186546890.25</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>43466</v>
-      </c>
-      <c r="B38">
-        <v>262387</v>
+        <v>40544</v>
+      </c>
+      <c r="B38" s="2">
+        <v>189329563.20999998</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>43497</v>
-      </c>
-      <c r="B39">
-        <v>262387</v>
+        <v>40575</v>
+      </c>
+      <c r="B39" s="2">
+        <v>189329563.20999998</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>43525</v>
-      </c>
-      <c r="B40">
-        <v>262387</v>
+        <v>40603</v>
+      </c>
+      <c r="B40" s="2">
+        <v>189329563.20999998</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>43556</v>
-      </c>
-      <c r="B41">
-        <v>262387</v>
+        <v>40634</v>
+      </c>
+      <c r="B41" s="2">
+        <v>189329563.20999998</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>43586</v>
-      </c>
-      <c r="B42">
-        <v>262387</v>
+        <v>40664</v>
+      </c>
+      <c r="B42" s="2">
+        <v>189329563.20999998</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>43617</v>
-      </c>
-      <c r="B43">
-        <v>262387</v>
+        <v>40695</v>
+      </c>
+      <c r="B43" s="2">
+        <v>189329563.20999998</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>43647</v>
-      </c>
-      <c r="B44">
-        <v>262387</v>
+        <v>40725</v>
+      </c>
+      <c r="B44" s="2">
+        <v>189329563.20999998</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>43678</v>
-      </c>
-      <c r="B45">
-        <v>262387</v>
+        <v>40756</v>
+      </c>
+      <c r="B45" s="2">
+        <v>189329563.20999998</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>43709</v>
-      </c>
-      <c r="B46">
-        <v>262387</v>
+        <v>40787</v>
+      </c>
+      <c r="B46" s="2">
+        <v>189329563.20999998</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
-        <v>43739</v>
-      </c>
-      <c r="B47">
-        <v>262387</v>
+        <v>40817</v>
+      </c>
+      <c r="B47" s="2">
+        <v>189329563.20999998</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
-        <v>43770</v>
-      </c>
-      <c r="B48">
-        <v>262387</v>
+        <v>40848</v>
+      </c>
+      <c r="B48" s="2">
+        <v>189329563.20999998</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
-        <v>43800</v>
-      </c>
-      <c r="B49">
-        <v>262387</v>
+        <v>40878</v>
+      </c>
+      <c r="B49" s="2">
+        <v>189329563.20999998</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
-        <v>43831</v>
-      </c>
-      <c r="B50">
-        <v>263764</v>
+        <v>40909</v>
+      </c>
+      <c r="B50" s="2">
+        <v>189304919.66</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
-        <v>43862</v>
-      </c>
-      <c r="B51">
-        <v>263764</v>
+        <v>40940</v>
+      </c>
+      <c r="B51" s="2">
+        <v>189304919.66</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
-        <v>43891</v>
-      </c>
-      <c r="B52">
-        <v>263764</v>
+        <v>40969</v>
+      </c>
+      <c r="B52" s="2">
+        <v>189304919.66</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
-        <v>43922</v>
-      </c>
-      <c r="B53">
-        <v>263764</v>
+        <v>41000</v>
+      </c>
+      <c r="B53" s="2">
+        <v>189304919.66</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
-        <v>43952</v>
-      </c>
-      <c r="B54">
-        <v>263764</v>
+        <v>41030</v>
+      </c>
+      <c r="B54" s="2">
+        <v>189304919.66</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
-        <v>43983</v>
-      </c>
-      <c r="B55">
-        <v>263764</v>
+        <v>41061</v>
+      </c>
+      <c r="B55" s="2">
+        <v>189304919.66</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
-        <v>44013</v>
-      </c>
-      <c r="B56">
-        <v>263764</v>
+        <v>41091</v>
+      </c>
+      <c r="B56" s="2">
+        <v>189304919.66</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
-        <v>44044</v>
-      </c>
-      <c r="B57">
-        <v>263764</v>
+        <v>41122</v>
+      </c>
+      <c r="B57" s="2">
+        <v>189304919.66</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
-        <v>44075</v>
-      </c>
-      <c r="B58">
-        <v>263764</v>
+        <v>41153</v>
+      </c>
+      <c r="B58" s="2">
+        <v>189304919.66</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
-        <v>44105</v>
-      </c>
-      <c r="B59">
-        <v>263764</v>
+        <v>41183</v>
+      </c>
+      <c r="B59" s="2">
+        <v>189304919.66</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
-        <v>44136</v>
-      </c>
-      <c r="B60">
-        <v>263764</v>
+        <v>41214</v>
+      </c>
+      <c r="B60" s="2">
+        <v>189304919.66</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
-        <v>44166</v>
-      </c>
-      <c r="B61">
-        <v>263764</v>
+        <v>41244</v>
+      </c>
+      <c r="B61" s="2">
+        <v>189304919.66</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
-        <v>44197</v>
-      </c>
-      <c r="B62">
-        <v>266756</v>
+        <v>41275</v>
+      </c>
+      <c r="B62" s="2">
+        <v>194922211.34999999</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
-        <v>44228</v>
-      </c>
-      <c r="B63">
-        <v>266756</v>
+        <v>41306</v>
+      </c>
+      <c r="B63" s="2">
+        <v>194922211.34999999</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
-        <v>44256</v>
-      </c>
-      <c r="B64">
-        <v>266756</v>
+        <v>41334</v>
+      </c>
+      <c r="B64" s="2">
+        <v>194922211.34999999</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
-        <v>44287</v>
-      </c>
-      <c r="B65">
-        <v>266756</v>
+        <v>41365</v>
+      </c>
+      <c r="B65" s="2">
+        <v>194922211.34999999</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
-        <v>44317</v>
-      </c>
-      <c r="B66">
-        <v>266756</v>
+        <v>41395</v>
+      </c>
+      <c r="B66" s="2">
+        <v>194922211.34999999</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
-        <v>44348</v>
-      </c>
-      <c r="B67">
-        <v>266756</v>
+        <v>41426</v>
+      </c>
+      <c r="B67" s="2">
+        <v>194922211.34999999</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
-        <v>44378</v>
-      </c>
-      <c r="B68">
-        <v>266756</v>
+        <v>41456</v>
+      </c>
+      <c r="B68" s="2">
+        <v>194922211.34999999</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
-        <v>44409</v>
-      </c>
-      <c r="B69">
-        <v>266756</v>
+        <v>41487</v>
+      </c>
+      <c r="B69" s="2">
+        <v>194922211.34999999</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
-        <v>44440</v>
-      </c>
-      <c r="B70">
-        <v>266756</v>
+        <v>41518</v>
+      </c>
+      <c r="B70" s="2">
+        <v>194922211.34999999</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
-        <v>44470</v>
-      </c>
-      <c r="B71">
-        <v>266756</v>
+        <v>41548</v>
+      </c>
+      <c r="B71" s="2">
+        <v>194922211.34999999</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
-        <v>44501</v>
-      </c>
-      <c r="B72">
-        <v>266756</v>
+        <v>41579</v>
+      </c>
+      <c r="B72" s="2">
+        <v>194922211.34999999</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
-        <v>44531</v>
-      </c>
-      <c r="B73">
-        <v>266756</v>
+        <v>41609</v>
+      </c>
+      <c r="B73" s="2">
+        <v>194922211.34999999</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
-        <v>44562</v>
-      </c>
-      <c r="B74">
-        <v>269482</v>
+        <v>41640</v>
+      </c>
+      <c r="B74" s="2">
+        <v>203143212.35999998</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
-        <v>44593</v>
-      </c>
-      <c r="B75">
-        <v>269482</v>
+        <v>41671</v>
+      </c>
+      <c r="B75" s="2">
+        <v>203143212.35999998</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
-        <v>44621</v>
-      </c>
-      <c r="B76">
-        <v>269482</v>
+        <v>41699</v>
+      </c>
+      <c r="B76" s="2">
+        <v>203143212.35999998</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
-        <v>44652</v>
-      </c>
-      <c r="B77">
-        <v>269482</v>
+        <v>41730</v>
+      </c>
+      <c r="B77" s="2">
+        <v>203143212.35999998</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
-        <v>44682</v>
-      </c>
-      <c r="B78">
-        <v>269482</v>
+        <v>41760</v>
+      </c>
+      <c r="B78" s="2">
+        <v>203143212.35999998</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
-        <v>44713</v>
-      </c>
-      <c r="B79">
-        <v>269482</v>
+        <v>41791</v>
+      </c>
+      <c r="B79" s="2">
+        <v>203143212.35999998</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
+        <v>41821</v>
+      </c>
+      <c r="B80" s="2">
+        <v>203143212.35999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>41852</v>
+      </c>
+      <c r="B81" s="2">
+        <v>203143212.35999998</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" s="1">
+        <v>41883</v>
+      </c>
+      <c r="B82" s="2">
+        <v>203143212.35999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" s="1">
+        <v>41913</v>
+      </c>
+      <c r="B83" s="2">
+        <v>203143212.35999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" s="1">
+        <v>41944</v>
+      </c>
+      <c r="B84" s="2">
+        <v>203143212.35999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="1">
+        <v>41974</v>
+      </c>
+      <c r="B85" s="2">
+        <v>203143212.35999998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" s="1">
+        <v>42005</v>
+      </c>
+      <c r="B86" s="2">
+        <v>209310645.70999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" s="1">
+        <v>42036</v>
+      </c>
+      <c r="B87" s="2">
+        <v>209310645.70999998</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" s="1">
+        <v>42064</v>
+      </c>
+      <c r="B88" s="2">
+        <v>209310645.70999998</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" s="1">
+        <v>42095</v>
+      </c>
+      <c r="B89" s="2">
+        <v>209310645.70999998</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" s="1">
+        <v>42125</v>
+      </c>
+      <c r="B90" s="2">
+        <v>209310645.70999998</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" s="1">
+        <v>42156</v>
+      </c>
+      <c r="B91" s="2">
+        <v>209310645.70999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" s="1">
+        <v>42186</v>
+      </c>
+      <c r="B92" s="2">
+        <v>209310645.70999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" s="1">
+        <v>42217</v>
+      </c>
+      <c r="B93" s="2">
+        <v>209310645.70999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="1">
+        <v>42248</v>
+      </c>
+      <c r="B94" s="2">
+        <v>209310645.70999998</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" s="1">
+        <v>42278</v>
+      </c>
+      <c r="B95" s="2">
+        <v>209310645.70999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" s="1">
+        <v>42309</v>
+      </c>
+      <c r="B96" s="2">
+        <v>209310645.70999998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" s="1">
+        <v>42339</v>
+      </c>
+      <c r="B97" s="2">
+        <v>209310645.70999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" s="1">
+        <v>42370</v>
+      </c>
+      <c r="B98" s="3">
+        <v>244131000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" s="1">
+        <v>42401</v>
+      </c>
+      <c r="B99" s="3">
+        <v>244131000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" s="1">
+        <v>42430</v>
+      </c>
+      <c r="B100" s="3">
+        <v>244131000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" s="1">
+        <v>42461</v>
+      </c>
+      <c r="B101" s="3">
+        <v>244131000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" s="1">
+        <v>42491</v>
+      </c>
+      <c r="B102" s="3">
+        <v>244131000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" s="1">
+        <v>42522</v>
+      </c>
+      <c r="B103" s="3">
+        <v>244131000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" s="1">
+        <v>42552</v>
+      </c>
+      <c r="B104" s="3">
+        <v>244131000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" s="1">
+        <v>42583</v>
+      </c>
+      <c r="B105" s="3">
+        <v>244131000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" s="1">
+        <v>42614</v>
+      </c>
+      <c r="B106" s="3">
+        <v>244131000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" s="1">
+        <v>42644</v>
+      </c>
+      <c r="B107" s="3">
+        <v>244131000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" s="1">
+        <v>42675</v>
+      </c>
+      <c r="B108" s="3">
+        <v>244131000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" s="1">
+        <v>42705</v>
+      </c>
+      <c r="B109" s="3">
+        <v>244131000</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" s="1">
+        <v>42736</v>
+      </c>
+      <c r="B110" s="3">
+        <v>249101000</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" s="1">
+        <v>42767</v>
+      </c>
+      <c r="B111" s="3">
+        <v>249101000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" s="1">
+        <v>42795</v>
+      </c>
+      <c r="B112" s="3">
+        <v>249101000</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="1">
+        <v>42826</v>
+      </c>
+      <c r="B113" s="3">
+        <v>249101000</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="1">
+        <v>42856</v>
+      </c>
+      <c r="B114" s="3">
+        <v>249101000</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" s="1">
+        <v>42887</v>
+      </c>
+      <c r="B115" s="3">
+        <v>249101000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" s="1">
+        <v>42917</v>
+      </c>
+      <c r="B116" s="3">
+        <v>249101000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" s="1">
+        <v>42948</v>
+      </c>
+      <c r="B117" s="3">
+        <v>249101000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" s="1">
+        <v>42979</v>
+      </c>
+      <c r="B118" s="3">
+        <v>249101000</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" s="1">
+        <v>43009</v>
+      </c>
+      <c r="B119" s="3">
+        <v>249101000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" s="1">
+        <v>43040</v>
+      </c>
+      <c r="B120" s="3">
+        <v>249101000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" s="1">
+        <v>43070</v>
+      </c>
+      <c r="B121" s="3">
+        <v>249101000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" s="1">
+        <v>43101</v>
+      </c>
+      <c r="B122" s="3">
+        <v>255861000</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" s="1">
+        <v>43132</v>
+      </c>
+      <c r="B123" s="3">
+        <v>255861000</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" s="1">
+        <v>43160</v>
+      </c>
+      <c r="B124" s="3">
+        <v>255861000</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" s="1">
+        <v>43191</v>
+      </c>
+      <c r="B125" s="3">
+        <v>255861000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" s="1">
+        <v>43221</v>
+      </c>
+      <c r="B126" s="3">
+        <v>255861000</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" s="1">
+        <v>43252</v>
+      </c>
+      <c r="B127" s="3">
+        <v>255861000</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" s="1">
+        <v>43282</v>
+      </c>
+      <c r="B128" s="3">
+        <v>255861000</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" s="1">
+        <v>43313</v>
+      </c>
+      <c r="B129" s="3">
+        <v>255861000</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" s="1">
+        <v>43344</v>
+      </c>
+      <c r="B130" s="3">
+        <v>255861000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" s="1">
+        <v>43374</v>
+      </c>
+      <c r="B131" s="3">
+        <v>255861000</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" s="1">
+        <v>43405</v>
+      </c>
+      <c r="B132" s="3">
+        <v>255861000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" s="1">
+        <v>43435</v>
+      </c>
+      <c r="B133" s="3">
+        <v>255861000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B134" s="3">
+        <v>262387000</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" s="1">
+        <v>43497</v>
+      </c>
+      <c r="B135" s="3">
+        <v>262387000</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" s="1">
+        <v>43525</v>
+      </c>
+      <c r="B136" s="3">
+        <v>262387000</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" s="1">
+        <v>43556</v>
+      </c>
+      <c r="B137" s="3">
+        <v>262387000</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" s="1">
+        <v>43586</v>
+      </c>
+      <c r="B138" s="3">
+        <v>262387000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" s="1">
+        <v>43617</v>
+      </c>
+      <c r="B139" s="3">
+        <v>262387000</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" s="1">
+        <v>43647</v>
+      </c>
+      <c r="B140" s="3">
+        <v>262387000</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" s="1">
+        <v>43678</v>
+      </c>
+      <c r="B141" s="3">
+        <v>262387000</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" s="1">
+        <v>43709</v>
+      </c>
+      <c r="B142" s="3">
+        <v>262387000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" s="1">
+        <v>43739</v>
+      </c>
+      <c r="B143" s="3">
+        <v>262387000</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" s="1">
+        <v>43770</v>
+      </c>
+      <c r="B144" s="3">
+        <v>262387000</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" s="1">
+        <v>43800</v>
+      </c>
+      <c r="B145" s="3">
+        <v>262387000</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B146" s="3">
+        <v>263764000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" s="1">
+        <v>43862</v>
+      </c>
+      <c r="B147" s="3">
+        <v>263764000</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" s="1">
+        <v>43891</v>
+      </c>
+      <c r="B148" s="3">
+        <v>263764000</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B149" s="3">
+        <v>263764000</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B150" s="3">
+        <v>263764000</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B151" s="3">
+        <v>263764000</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B152" s="3">
+        <v>263764000</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B153" s="3">
+        <v>263764000</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B154" s="3">
+        <v>263764000</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B155" s="3">
+        <v>263764000</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B156" s="3">
+        <v>263764000</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B157" s="3">
+        <v>263764000</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B158" s="3">
+        <v>266756000</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A159" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B159" s="3">
+        <v>266756000</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A160" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B160" s="3">
+        <v>266756000</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A161" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B161" s="3">
+        <v>266756000</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A162" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B162" s="3">
+        <v>266756000</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A163" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B163" s="3">
+        <v>266756000</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A164" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B164" s="3">
+        <v>266756000</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A165" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B165" s="3">
+        <v>266756000</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A166" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B166" s="3">
+        <v>266756000</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A167" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B167" s="3">
+        <v>266756000</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A168" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B168" s="3">
+        <v>266756000</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A169" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B169" s="3">
+        <v>266756000</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A170" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B170" s="3">
+        <v>269482000</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A171" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B171" s="3">
+        <v>269482000</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A172" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B172" s="3">
+        <v>269482000</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A173" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B173" s="3">
+        <v>269482000</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A174" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B174" s="3">
+        <v>269482000</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A175" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B175" s="3">
+        <v>269482000</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A176" s="1">
         <v>44743</v>
       </c>
-      <c r="B80">
-        <v>269482</v>
+      <c r="B176" s="3">
+        <v>269482000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>